<commit_message>
fix count of items
</commit_message>
<xml_diff>
--- a/Examples/newitems.xlsx
+++ b/Examples/newitems.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\Excel_Combine_And_Sort\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2816EBD-72E0-4520-A5C9-2F02DC275D28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Downlinks" sheetId="1" r:id="rId1"/>
@@ -20,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Site</t>
   </si>
@@ -70,12 +65,15 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,7 +418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -546,12 +544,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A4" sqref="A4:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,103 +565,114 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>43</v>
-      </c>
-      <c r="J3" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>564</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>453</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>564</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>453</v>
       </c>
       <c r="J7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>77</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>45</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>4</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J12" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>56</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix multiple date items
</commit_message>
<xml_diff>
--- a/Examples/newitems.xlsx
+++ b/Examples/newitems.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\Excel_Combine_And_Sort\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2816EBD-72E0-4520-A5C9-2F02DC275D28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Downlinks" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Site</t>
   </si>
@@ -68,12 +67,15 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>adfasdfas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -544,12 +546,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +677,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>222</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>